<commit_message>
Dividend Testing - Error
</commit_message>
<xml_diff>
--- a/Balance.xlsx
+++ b/Balance.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mailk\codes\Monopoly-Shares\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manav\OneDrive\Documents\Monopoly Shares\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D8508A-FAB2-44E1-92CA-101F04E16D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F15BDED-5332-48AA-A68C-021B36B38A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -76,6 +76,9 @@
     <t>Turns Played</t>
   </si>
   <si>
+    <t>Dividend Payout Ratio</t>
+  </si>
+  <si>
     <t>Debt Taken</t>
   </si>
   <si>
@@ -110,9 +113,6 @@
   </si>
   <si>
     <t>Player 5 Shares</t>
-  </si>
-  <si>
-    <t>Dividend Payout Ratio</t>
   </si>
 </sst>
 </file>
@@ -487,7 +487,7 @@
   <dimension ref="A3:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -545,7 +545,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -642,19 +642,19 @@
         <v>16</v>
       </c>
       <c r="B10">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D10">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E10">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F10">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -662,24 +662,24 @@
         <v>17</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B12">
         <v>0.1</v>
@@ -699,13 +699,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -719,13 +719,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -739,7 +739,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B16">
         <v>5</v>
@@ -759,7 +759,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17">
         <v>0.5</v>
@@ -779,27 +779,27 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B22">
         <v>100</v>
@@ -819,7 +819,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -839,7 +839,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -859,7 +859,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -879,7 +879,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B26">
         <v>0</v>

</xml_diff>

<commit_message>
Fixed share holding implementation
While it works fine, it is not replayable
So if your log has new transactions
It cannot give you an accurate answer for prev round
</commit_message>
<xml_diff>
--- a/Balance.xlsx
+++ b/Balance.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manav\OneDrive\Documents\Monopoly Shares\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mailk\codes\Monopoly-Shares\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239EE919-27FF-46ED-8F10-A045F7437691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90E5500-E811-4EAA-84BC-F0FEF694B174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -487,7 +487,7 @@
   <dimension ref="A3:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -545,7 +545,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -705,7 +705,7 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -725,7 +725,7 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D15">
         <v>0</v>

</xml_diff>